<commit_message>
add afsk300 numbers to xl
</commit_message>
<xml_diff>
--- a/LoopIntegralReference copy.xlsx
+++ b/LoopIntegralReference copy.xlsx
@@ -4,13 +4,14 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="7815" yWindow="45" windowWidth="20940" windowHeight="16995"/>
+    <workbookView xWindow="7815" yWindow="45" windowWidth="20940" windowHeight="16995" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Modified Costas Loop" sheetId="4" r:id="rId1"/>
     <sheet name="Traditional Costas Loop" sheetId="1" r:id="rId2"/>
     <sheet name="Costas Loop Gain" sheetId="2" r:id="rId3"/>
     <sheet name="AttackDecay" sheetId="3" r:id="rId4"/>
+    <sheet name="AFSK PLL" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="125725"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="39">
   <si>
     <t>BPSK 300</t>
   </si>
@@ -144,6 +145,9 @@
   </si>
   <si>
     <t>Count/Sample</t>
+  </si>
+  <si>
+    <t>AFSKPLL 300</t>
   </si>
 </sst>
 </file>
@@ -598,7 +602,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L72"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A37" workbookViewId="0">
       <selection activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
@@ -3239,4 +3243,144 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:J6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="15.75" thickBot="1">
+      <c r="A1" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="3">
+        <v>65536</v>
+      </c>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="5"/>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3">
+        <v>14400</v>
+      </c>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="8"/>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="6"/>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4">
+        <v>20</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4">
+        <v>15</v>
+      </c>
+      <c r="J4" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="6"/>
+      <c r="B5">
+        <v>1.2E-4</v>
+      </c>
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+      <c r="J5" s="9"/>
+    </row>
+    <row r="6" spans="1:10" ht="15.75" thickBot="1">
+      <c r="A6" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="11">
+        <v>1.2E-4</v>
+      </c>
+      <c r="C6" s="11">
+        <f>ROUND(POWER(2,$C$4)*B6, 0)</f>
+        <v>126</v>
+      </c>
+      <c r="D6" s="11">
+        <v>0.3</v>
+      </c>
+      <c r="E6" s="11">
+        <f>ROUND(POWER(2,$E4)*D6, 0)</f>
+        <v>9830</v>
+      </c>
+      <c r="F6" s="11">
+        <v>50</v>
+      </c>
+      <c r="G6" s="12">
+        <v>0.5</v>
+      </c>
+      <c r="H6" s="11">
+        <f>ROUND(((F6*(1+G6)) * $B2/$B3)/B6, 0)</f>
+        <v>2844444</v>
+      </c>
+      <c r="I6" s="11">
+        <v>0.9</v>
+      </c>
+      <c r="J6" s="13">
+        <f>LOG(H6*C6,2)</f>
+        <v>28.4169951710733</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:J1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add afsk 300 pll filter calcs to xl
</commit_message>
<xml_diff>
--- a/LoopIntegralReference copy.xlsx
+++ b/LoopIntegralReference copy.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="7815" yWindow="45" windowWidth="20940" windowHeight="16995" activeTab="4"/>
+    <workbookView xWindow="7815" yWindow="45" windowWidth="20940" windowHeight="16995" firstSheet="2" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Modified Costas Loop" sheetId="4" r:id="rId1"/>
@@ -3250,7 +3250,7 @@
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>

</xml_diff>